<commit_message>
Wide version of OTA slide.
</commit_message>
<xml_diff>
--- a/Output/OTA/DoD_Acq_Trends_OTA.xlsx
+++ b/Output/OTA/DoD_Acq_Trends_OTA.xlsx
@@ -129,10 +129,10 @@
     <numFmt numFmtId="179" formatCode="0.00,,,&quot;B&quot;"/>
     <numFmt numFmtId="178" formatCode="0.00,,,&quot;B&quot;"/>
     <numFmt numFmtId="181" formatCode="0.00,,,&quot;B&quot;"/>
-    <numFmt numFmtId="185" formatCode="0.00,,,&quot;B&quot;"/>
+    <numFmt numFmtId="186" formatCode="0.00,,,&quot;B&quot;"/>
     <numFmt numFmtId="176" formatCode="0.00,,,&quot;B&quot;"/>
     <numFmt numFmtId="180" formatCode="0.00,,,&quot;B&quot;"/>
-    <numFmt numFmtId="186" formatCode="0.00,,,&quot;B&quot;"/>
+    <numFmt numFmtId="187" formatCode="0.00,,,&quot;B&quot;"/>
   </numFmts>
   <fonts count="2">
     <font>
@@ -173,10 +173,10 @@
     <xf numFmtId="179" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyNumberFormat="1"/>
     <xf numFmtId="178" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyNumberFormat="1"/>
     <xf numFmtId="181" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyNumberFormat="1"/>
-    <xf numFmtId="185" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyNumberFormat="1"/>
+    <xf numFmtId="186" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyNumberFormat="1"/>
     <xf numFmtId="176" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyNumberFormat="1"/>
     <xf numFmtId="180" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyNumberFormat="1"/>
-    <xf numFmtId="186" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyNumberFormat="1"/>
+    <xf numFmtId="187" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>

</xml_diff>

<commit_message>
Trying again to sync up after PBL work and kludge.
</commit_message>
<xml_diff>
--- a/Output/OTA/DoD_Acq_Trends_OTA.xlsx
+++ b/Output/OTA/DoD_Acq_Trends_OTA.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
   <si>
     <t xml:space="preserve">TypeOfAgreement</t>
   </si>
@@ -119,6 +119,12 @@
   </si>
   <si>
     <t xml:space="preserve">PROTOTYPE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2011</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2012</t>
   </si>
 </sst>
 </file>
@@ -129,10 +135,10 @@
     <numFmt numFmtId="179" formatCode="0.00,,,&quot;B&quot;"/>
     <numFmt numFmtId="178" formatCode="0.00,,,&quot;B&quot;"/>
     <numFmt numFmtId="181" formatCode="0.00,,,&quot;B&quot;"/>
-    <numFmt numFmtId="193" formatCode="0.00,,,&quot;B&quot;"/>
+    <numFmt numFmtId="198" formatCode="0.00,,,&quot;B&quot;"/>
     <numFmt numFmtId="180" formatCode="0.00,,,&quot;B&quot;"/>
     <numFmt numFmtId="191" formatCode="0.00,,,&quot;B&quot;"/>
-    <numFmt numFmtId="194" formatCode="0.00,,,&quot;B&quot;"/>
+    <numFmt numFmtId="199" formatCode="0.00,,,&quot;B&quot;"/>
   </numFmts>
   <fonts count="2">
     <font>
@@ -173,10 +179,10 @@
     <xf numFmtId="179" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyNumberFormat="1"/>
     <xf numFmtId="178" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyNumberFormat="1"/>
     <xf numFmtId="181" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyNumberFormat="1"/>
-    <xf numFmtId="193" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyNumberFormat="1"/>
+    <xf numFmtId="198" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyNumberFormat="1"/>
     <xf numFmtId="180" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyNumberFormat="1"/>
     <xf numFmtId="191" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyNumberFormat="1"/>
-    <xf numFmtId="194" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyNumberFormat="1"/>
+    <xf numFmtId="199" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -696,39 +702,45 @@
         <v>0</v>
       </c>
       <c r="N1" t="s">
+        <v>35</v>
+      </c>
+      <c r="O1" t="s">
+        <v>36</v>
+      </c>
+      <c r="P1" t="s">
         <v>1</v>
       </c>
-      <c r="O1" t="s">
+      <c r="Q1" t="s">
         <v>2</v>
       </c>
-      <c r="P1" t="s">
+      <c r="R1" t="s">
         <v>3</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="S1" t="s">
         <v>4</v>
       </c>
-      <c r="R1" t="s">
+      <c r="T1" t="s">
         <v>5</v>
       </c>
-      <c r="S1" t="s">
+      <c r="U1" t="s">
         <v>6</v>
       </c>
-      <c r="T1" t="s">
+      <c r="V1" t="s">
         <v>7</v>
       </c>
-      <c r="U1" t="s">
+      <c r="W1" t="s">
         <v>8</v>
       </c>
-      <c r="V1" t="s">
+      <c r="X1" t="s">
         <v>9</v>
       </c>
-      <c r="W1" t="s">
+      <c r="Y1" t="s">
         <v>10</v>
       </c>
-      <c r="X1" t="s">
+      <c r="Z1" t="s">
         <v>11</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="AA1" t="s">
         <v>12</v>
       </c>
     </row>
@@ -746,42 +758,48 @@
         <v>13</v>
       </c>
       <c r="N2" s="7" t="n">
+        <v>265546547.95</v>
+      </c>
+      <c r="O2" s="7" t="n">
+        <v>417275713.03</v>
+      </c>
+      <c r="P2" s="7" t="n">
         <v>305798391.22</v>
       </c>
-      <c r="O2" s="7" t="n">
+      <c r="Q2" s="7" t="n">
         <v>467083660.6</v>
       </c>
-      <c r="P2" s="7" t="n">
+      <c r="R2" s="7" t="n">
         <v>623306976.79</v>
       </c>
-      <c r="Q2" s="7" t="n">
+      <c r="S2" s="7" t="n">
         <v>902166349.31</v>
       </c>
-      <c r="R2" s="7" t="n">
+      <c r="T2" s="7" t="n">
         <v>1545404234.55</v>
       </c>
-      <c r="S2" s="7" t="n">
+      <c r="U2" s="7" t="n">
         <v>2947049116.68</v>
       </c>
-      <c r="T2" s="7" t="n">
-        <v>4946987294.07</v>
-      </c>
-      <c r="U2" s="7" t="n">
-        <v>13038972855.76</v>
-      </c>
       <c r="V2" s="7" t="n">
-        <v>9791890070.47</v>
+        <v>4946319047.07</v>
       </c>
       <c r="W2" s="7" t="n">
-        <v>5526836631.66</v>
+        <v>13032740676.7</v>
       </c>
       <c r="X2" s="7" t="n">
-        <v>5551948646.64</v>
+        <v>9791966578.47</v>
       </c>
       <c r="Y2" s="7" t="n">
-        <v>900528444.88</v>
-      </c>
-      <c r="Z2" s="7"/>
+        <v>5519807774.6</v>
+      </c>
+      <c r="Z2" s="7" t="n">
+        <v>5565329170.95</v>
+      </c>
+      <c r="AA2" s="7" t="n">
+        <v>932467858.03</v>
+      </c>
+      <c r="AB2" s="7"/>
     </row>
     <row r="3">
       <c r="A3" t="str">
@@ -802,25 +820,27 @@
       <c r="Q3" s="7"/>
       <c r="R3" s="7"/>
       <c r="S3" s="7"/>
-      <c r="T3" s="7" t="n">
+      <c r="T3" s="7"/>
+      <c r="U3" s="7"/>
+      <c r="V3" s="7" t="n">
         <v>348308</v>
       </c>
-      <c r="U3" s="7" t="n">
+      <c r="W3" s="7" t="n">
         <v>229376133.84</v>
       </c>
-      <c r="V3" s="7" t="n">
+      <c r="X3" s="7" t="n">
         <v>763694993.38</v>
       </c>
-      <c r="W3" s="7" t="n">
+      <c r="Y3" s="7" t="n">
         <v>571942623.76</v>
       </c>
-      <c r="X3" s="7" t="n">
-        <v>1420811414.95</v>
-      </c>
-      <c r="Y3" s="7" t="n">
-        <v>134979795.75</v>
-      </c>
-      <c r="Z3" s="7"/>
+      <c r="Z3" s="7" t="n">
+        <v>1471331710.26</v>
+      </c>
+      <c r="AA3" s="7" t="n">
+        <v>150693771.27</v>
+      </c>
+      <c r="AB3" s="7"/>
     </row>
     <row r="4">
       <c r="A4" t="str">
@@ -835,43 +855,45 @@
       <c r="M4" t="s">
         <v>13</v>
       </c>
-      <c r="N4" s="7" t="n">
+      <c r="N4" s="7"/>
+      <c r="O4" s="7"/>
+      <c r="P4" s="7" t="n">
         <v>1087637</v>
       </c>
-      <c r="O4" s="7" t="n">
+      <c r="Q4" s="7" t="n">
         <v>2694831</v>
       </c>
-      <c r="P4" s="7" t="n">
+      <c r="R4" s="7" t="n">
         <v>2316363</v>
       </c>
-      <c r="Q4" s="7" t="n">
+      <c r="S4" s="7" t="n">
         <v>4928841</v>
       </c>
-      <c r="R4" s="7" t="n">
+      <c r="T4" s="7" t="n">
         <v>50000</v>
       </c>
-      <c r="S4" s="7" t="n">
+      <c r="U4" s="7" t="n">
         <v>31955707.71</v>
       </c>
-      <c r="T4" s="7" t="n">
+      <c r="V4" s="7" t="n">
         <v>167767241.67</v>
       </c>
-      <c r="U4" s="7" t="n">
+      <c r="W4" s="7" t="n">
         <v>621072980.27</v>
       </c>
-      <c r="V4" s="7" t="n">
-        <v>946299367.02</v>
-      </c>
-      <c r="W4" s="7" t="n">
-        <v>1392818930.33</v>
-      </c>
       <c r="X4" s="7" t="n">
-        <v>2396228169.59</v>
+        <v>946510457.02</v>
       </c>
       <c r="Y4" s="7" t="n">
-        <v>287480377.3</v>
-      </c>
-      <c r="Z4" s="7"/>
+        <v>1392865308.59</v>
+      </c>
+      <c r="Z4" s="7" t="n">
+        <v>2397333089.99</v>
+      </c>
+      <c r="AA4" s="7" t="n">
+        <v>295278531.69</v>
+      </c>
+      <c r="AB4" s="7"/>
     </row>
     <row r="5">
       <c r="A5" t="str">
@@ -893,22 +915,24 @@
       <c r="R5" s="7"/>
       <c r="S5" s="7"/>
       <c r="T5" s="7"/>
-      <c r="U5" s="7" t="n">
+      <c r="U5" s="7"/>
+      <c r="V5" s="7"/>
+      <c r="W5" s="7" t="n">
         <v>10203844.83</v>
       </c>
-      <c r="V5" s="7" t="n">
+      <c r="X5" s="7" t="n">
         <v>37345087.25</v>
       </c>
-      <c r="W5" s="7" t="n">
+      <c r="Y5" s="7" t="n">
         <v>80559943.51</v>
       </c>
-      <c r="X5" s="7" t="n">
+      <c r="Z5" s="7" t="n">
         <v>213676422.24</v>
       </c>
-      <c r="Y5" s="7" t="n">
-        <v>42162701.4</v>
-      </c>
-      <c r="Z5" s="7"/>
+      <c r="AA5" s="7" t="n">
+        <v>44660062.4</v>
+      </c>
+      <c r="AB5" s="7"/>
     </row>
     <row r="6">
       <c r="A6" t="str">
@@ -924,42 +948,48 @@
         <v>13</v>
       </c>
       <c r="N6" s="7" t="n">
+        <v>195000</v>
+      </c>
+      <c r="O6" s="7" t="n">
+        <v>1897530</v>
+      </c>
+      <c r="P6" s="7" t="n">
         <v>3903539</v>
       </c>
-      <c r="O6" s="7" t="n">
+      <c r="Q6" s="7" t="n">
         <v>4636181</v>
       </c>
-      <c r="P6" s="7" t="n">
+      <c r="R6" s="7" t="n">
         <v>4993631</v>
       </c>
-      <c r="Q6" s="7" t="n">
+      <c r="S6" s="7" t="n">
         <v>250037783</v>
       </c>
-      <c r="R6" s="7" t="n">
+      <c r="T6" s="7" t="n">
         <v>187693198</v>
       </c>
-      <c r="S6" s="7" t="n">
+      <c r="U6" s="7" t="n">
         <v>526509339.38</v>
       </c>
-      <c r="T6" s="7" t="n">
+      <c r="V6" s="7" t="n">
         <v>1428461728.3</v>
       </c>
-      <c r="U6" s="7" t="n">
-        <v>1358409639.11</v>
-      </c>
-      <c r="V6" s="7" t="n">
-        <v>1922431021.18</v>
-      </c>
       <c r="W6" s="7" t="n">
-        <v>1373770303.73</v>
+        <v>1359909639.11</v>
       </c>
       <c r="X6" s="7" t="n">
-        <v>2582227987.89</v>
+        <v>1922436021.18</v>
       </c>
       <c r="Y6" s="7" t="n">
-        <v>1081080934.21</v>
-      </c>
-      <c r="Z6" s="7"/>
+        <v>1375470303.73</v>
+      </c>
+      <c r="Z6" s="7" t="n">
+        <v>2602963536.89</v>
+      </c>
+      <c r="AA6" s="7" t="n">
+        <v>1194000298.8</v>
+      </c>
+      <c r="AB6" s="7"/>
     </row>
     <row r="7">
       <c r="A7" t="str">
@@ -981,22 +1011,24 @@
       <c r="R7" s="7"/>
       <c r="S7" s="7"/>
       <c r="T7" s="7"/>
-      <c r="U7" s="7" t="n">
+      <c r="U7" s="7"/>
+      <c r="V7" s="7"/>
+      <c r="W7" s="7" t="n">
         <v>76299804.16</v>
       </c>
-      <c r="V7" s="7" t="n">
+      <c r="X7" s="7" t="n">
         <v>62117307.39</v>
       </c>
-      <c r="W7" s="7" t="n">
+      <c r="Y7" s="7" t="n">
         <v>61769399.21</v>
       </c>
-      <c r="X7" s="7" t="n">
+      <c r="Z7" s="7" t="n">
         <v>107150475.74</v>
       </c>
-      <c r="Y7" s="7" t="n">
-        <v>31352988.8</v>
-      </c>
-      <c r="Z7" s="7"/>
+      <c r="AA7" s="7" t="n">
+        <v>33643822.15</v>
+      </c>
+      <c r="AB7" s="7"/>
     </row>
     <row r="8">
       <c r="A8" t="str">
@@ -1016,14 +1048,16 @@
       <c r="R8" s="7"/>
       <c r="S8" s="7"/>
       <c r="T8" s="7"/>
-      <c r="U8" s="7" t="n">
+      <c r="U8" s="7"/>
+      <c r="V8" s="7"/>
+      <c r="W8" s="7" t="n">
         <v>235000</v>
       </c>
-      <c r="V8" s="7"/>
-      <c r="W8" s="7"/>
       <c r="X8" s="7"/>
       <c r="Y8" s="7"/>
       <c r="Z8" s="7"/>
+      <c r="AA8" s="7"/>
+      <c r="AB8" s="7"/>
     </row>
     <row r="9">
       <c r="A9" t="str">
@@ -1047,16 +1081,18 @@
       <c r="T9" s="7"/>
       <c r="U9" s="7"/>
       <c r="V9" s="7"/>
-      <c r="W9" s="7" t="n">
+      <c r="W9" s="7"/>
+      <c r="X9" s="7"/>
+      <c r="Y9" s="7" t="n">
         <v>623617676</v>
       </c>
-      <c r="X9" s="7" t="n">
-        <v>1151457876.22</v>
-      </c>
-      <c r="Y9" s="7" t="n">
+      <c r="Z9" s="7" t="n">
+        <v>1153957876.22</v>
+      </c>
+      <c r="AA9" s="7" t="n">
         <v>205871368</v>
       </c>
-      <c r="Z9" s="7"/>
+      <c r="AB9" s="7"/>
     </row>
     <row r="10">
       <c r="A10" t="str">
@@ -1078,22 +1114,24 @@
       <c r="R10" s="7"/>
       <c r="S10" s="7"/>
       <c r="T10" s="7"/>
-      <c r="U10" s="7" t="n">
+      <c r="U10" s="7"/>
+      <c r="V10" s="7"/>
+      <c r="W10" s="7" t="n">
         <v>79948980</v>
       </c>
-      <c r="V10" s="7" t="n">
+      <c r="X10" s="7" t="n">
         <v>160693402</v>
       </c>
-      <c r="W10" s="7" t="n">
+      <c r="Y10" s="7" t="n">
         <v>232946539</v>
       </c>
-      <c r="X10" s="7" t="n">
+      <c r="Z10" s="7" t="n">
         <v>421174933.8</v>
       </c>
-      <c r="Y10" s="7" t="n">
+      <c r="AA10" s="7" t="n">
         <v>48319960</v>
       </c>
-      <c r="Z10" s="7"/>
+      <c r="AB10" s="7"/>
     </row>
     <row r="11">
       <c r="A11" t="str">
@@ -1116,19 +1154,21 @@
       <c r="S11" s="7"/>
       <c r="T11" s="7"/>
       <c r="U11" s="7"/>
-      <c r="V11" s="7" t="n">
+      <c r="V11" s="7"/>
+      <c r="W11" s="7"/>
+      <c r="X11" s="7" t="n">
         <v>3500000</v>
       </c>
-      <c r="W11" s="7" t="n">
+      <c r="Y11" s="7" t="n">
         <v>6155000</v>
       </c>
-      <c r="X11" s="7" t="n">
+      <c r="Z11" s="7" t="n">
         <v>8050000</v>
       </c>
-      <c r="Y11" s="7" t="n">
+      <c r="AA11" s="7" t="n">
         <v>2500000</v>
       </c>
-      <c r="Z11" s="7"/>
+      <c r="AB11" s="7"/>
     </row>
     <row r="12">
       <c r="A12" t="str">
@@ -1144,42 +1184,48 @@
         <v>13</v>
       </c>
       <c r="N12" s="7" t="n">
+        <v>61502552</v>
+      </c>
+      <c r="O12" s="7" t="n">
+        <v>38758780</v>
+      </c>
+      <c r="P12" s="7" t="n">
         <v>22014936</v>
       </c>
-      <c r="O12" s="7" t="n">
+      <c r="Q12" s="7" t="n">
         <v>40849581</v>
       </c>
-      <c r="P12" s="7" t="n">
+      <c r="R12" s="7" t="n">
         <v>62907051</v>
       </c>
-      <c r="Q12" s="7" t="n">
+      <c r="S12" s="7" t="n">
         <v>214782354.78</v>
       </c>
-      <c r="R12" s="7" t="n">
+      <c r="T12" s="7" t="n">
         <v>379711068.32</v>
       </c>
-      <c r="S12" s="7" t="n">
+      <c r="U12" s="7" t="n">
         <v>377879847.47</v>
       </c>
-      <c r="T12" s="7" t="n">
+      <c r="V12" s="7" t="n">
         <v>423307981.86</v>
       </c>
-      <c r="U12" s="7" t="n">
+      <c r="W12" s="7" t="n">
         <v>354104917.18</v>
       </c>
-      <c r="V12" s="7" t="n">
+      <c r="X12" s="7" t="n">
         <v>347468914.34</v>
       </c>
-      <c r="W12" s="7" t="n">
+      <c r="Y12" s="7" t="n">
         <v>312343199.61</v>
       </c>
-      <c r="X12" s="7" t="n">
+      <c r="Z12" s="7" t="n">
         <v>469335440.28</v>
       </c>
-      <c r="Y12" s="7" t="n">
+      <c r="AA12" s="7" t="n">
         <v>130386939.07</v>
       </c>
-      <c r="Z12" s="7"/>
+      <c r="AB12" s="7"/>
     </row>
     <row r="13">
       <c r="A13" t="str">
@@ -1204,13 +1250,15 @@
       <c r="U13" s="7"/>
       <c r="V13" s="7"/>
       <c r="W13" s="7"/>
-      <c r="X13" s="7" t="n">
+      <c r="X13" s="7"/>
+      <c r="Y13" s="7"/>
+      <c r="Z13" s="7" t="n">
         <v>6065329.49</v>
       </c>
-      <c r="Y13" s="7" t="n">
+      <c r="AA13" s="7" t="n">
         <v>3293394</v>
       </c>
-      <c r="Z13" s="7"/>
+      <c r="AB13" s="7"/>
     </row>
     <row r="14">
       <c r="A14" t="str">
@@ -1226,42 +1274,48 @@
         <v>13</v>
       </c>
       <c r="N14" s="7" t="n">
+        <v>65790468.88</v>
+      </c>
+      <c r="O14" s="7" t="n">
+        <v>16073573.33</v>
+      </c>
+      <c r="P14" s="7" t="n">
         <v>7755269.51</v>
       </c>
-      <c r="O14" s="7" t="n">
+      <c r="Q14" s="7" t="n">
         <v>8294831</v>
       </c>
-      <c r="P14" s="7" t="n">
+      <c r="R14" s="7" t="n">
         <v>1359295.89</v>
       </c>
-      <c r="Q14" s="7" t="n">
+      <c r="S14" s="7" t="n">
         <v>61241002.21</v>
       </c>
-      <c r="R14" s="7" t="n">
+      <c r="T14" s="7" t="n">
         <v>2629821</v>
       </c>
-      <c r="S14" s="7" t="n">
+      <c r="U14" s="7" t="n">
         <v>70515217.94</v>
       </c>
-      <c r="T14" s="7" t="n">
+      <c r="V14" s="7" t="n">
         <v>243888265.92</v>
       </c>
-      <c r="U14" s="7" t="n">
+      <c r="W14" s="7" t="n">
         <v>525334651.5</v>
       </c>
-      <c r="V14" s="7" t="n">
-        <v>418465604.4</v>
-      </c>
-      <c r="W14" s="7" t="n">
-        <v>508547161.27</v>
-      </c>
       <c r="X14" s="7" t="n">
-        <v>1025345573.13</v>
+        <v>418397828.4</v>
       </c>
       <c r="Y14" s="7" t="n">
-        <v>174609780.59</v>
-      </c>
-      <c r="Z14" s="7"/>
+        <v>510989564.27</v>
+      </c>
+      <c r="Z14" s="7" t="n">
+        <v>1035745802.06</v>
+      </c>
+      <c r="AA14" s="7" t="n">
+        <v>179010264.98</v>
+      </c>
+      <c r="AB14" s="7"/>
     </row>
     <row r="15">
       <c r="A15" t="str">
@@ -1282,25 +1336,27 @@
       <c r="Q15" s="7"/>
       <c r="R15" s="7"/>
       <c r="S15" s="7"/>
-      <c r="T15" s="7" t="n">
+      <c r="T15" s="7"/>
+      <c r="U15" s="7"/>
+      <c r="V15" s="7" t="n">
         <v>655268.97</v>
       </c>
-      <c r="U15" s="7" t="n">
+      <c r="W15" s="7" t="n">
         <v>41181902.47</v>
       </c>
-      <c r="V15" s="7" t="n">
+      <c r="X15" s="7" t="n">
         <v>212840425.61</v>
       </c>
-      <c r="W15" s="7" t="n">
-        <v>289330105.34</v>
-      </c>
-      <c r="X15" s="7" t="n">
+      <c r="Y15" s="7" t="n">
+        <v>289268271.34</v>
+      </c>
+      <c r="Z15" s="7" t="n">
         <v>327031127.28</v>
       </c>
-      <c r="Y15" s="7" t="n">
+      <c r="AA15" s="7" t="n">
         <v>83820685.66</v>
       </c>
-      <c r="Z15" s="7"/>
+      <c r="AB15" s="7"/>
     </row>
     <row r="16">
       <c r="A16" t="str">
@@ -1351,7 +1407,13 @@
       <c r="Y16" s="7" t="str">
         <f>Sum(Y2:Y15)</f>
       </c>
-      <c r="Z16" s="7"/>
+      <c r="Z16" s="7" t="str">
+        <f>Sum(Z2:Z15)</f>
+      </c>
+      <c r="AA16" s="7" t="str">
+        <f>Sum(AA2:AA15)</f>
+      </c>
+      <c r="AB16" s="7"/>
     </row>
     <row r="17">
       <c r="A17" t="str">

</xml_diff>